<commit_message>
Updates to the spreadsheet to rename some scenarios
</commit_message>
<xml_diff>
--- a/Scenario_Schedule_spreadsheet/Scenario Schedule for Care Connect NHS 111 UEC Booking.xlsx
+++ b/Scenario_Schedule_spreadsheet/Scenario Schedule for Care Connect NHS 111 UEC Booking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Technical_Specialist_Folder\NHS_111_UEC_Booking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\TKW-5.0.5\TKW\config\FHIR_111_UEC\Scenario_Schedule_spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A78BBA-F290-4CBB-8DDA-C767ACA8A2D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A881FA2-0E1A-4190-A786-7C4DCDC03BF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14145" xr2:uid="{47186762-2036-4FBA-BFCD-4F22E763EBB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14760" xr2:uid="{47186762-2036-4FBA-BFCD-4F22E763EBB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Provider Simulator" sheetId="1" r:id="rId1"/>
@@ -668,9 +668,6 @@
     <t>CancelAppointment_UnsupportedMediaType</t>
   </si>
   <si>
-    <t>CancelAppointment_BadGateway</t>
-  </si>
-  <si>
     <t>Should we be returning Date in all headers? As we do in ReasonableAdjustments</t>
   </si>
   <si>
@@ -708,6 +705,9 @@
   </si>
   <si>
     <t>Column7</t>
+  </si>
+  <si>
+    <t>CancelAppointment_Invalid</t>
   </si>
 </sst>
 </file>
@@ -1177,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFDA31F-0014-4FDB-8F0D-993366C26DC7}">
   <dimension ref="B2:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H28" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,7 +1480,7 @@
         <v>162</v>
       </c>
       <c r="H10" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" ref="H10:H22" si="0">$C$4</f>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I10" t="s">
@@ -1514,7 +1514,7 @@
         <v>182</v>
       </c>
       <c r="H11" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I11" t="s">
@@ -1548,7 +1548,7 @@
         <v>183</v>
       </c>
       <c r="H12" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I12" t="s">
@@ -1582,7 +1582,7 @@
         <v>184</v>
       </c>
       <c r="H13" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I13" t="s">
@@ -1616,7 +1616,7 @@
         <v>185</v>
       </c>
       <c r="H14" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I14" t="s">
@@ -1650,7 +1650,7 @@
         <v>186</v>
       </c>
       <c r="H15" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I15" t="s">
@@ -1684,7 +1684,7 @@
         <v>187</v>
       </c>
       <c r="H16" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I16" t="s">
@@ -1718,7 +1718,7 @@
         <v>188</v>
       </c>
       <c r="H17" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I17" t="s">
@@ -1752,7 +1752,7 @@
         <v>166</v>
       </c>
       <c r="H18" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I18" t="s">
@@ -1788,7 +1788,7 @@
         <v>167</v>
       </c>
       <c r="H19" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I19" t="s">
@@ -1822,7 +1822,7 @@
         <v>168</v>
       </c>
       <c r="H20" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I20" t="s">
@@ -1856,7 +1856,7 @@
         <v>169</v>
       </c>
       <c r="H21" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I21" t="s">
@@ -1890,7 +1890,7 @@
         <v>176</v>
       </c>
       <c r="H22" s="6" t="str">
-        <f>$C$4</f>
+        <f t="shared" si="0"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I22" t="s">
@@ -1924,7 +1924,7 @@
         <v>180</v>
       </c>
       <c r="H23" s="6" t="str">
-        <f t="shared" ref="H23:H24" si="0">$C$4</f>
+        <f t="shared" ref="H23:H24" si="1">$C$4</f>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I23" t="s">
@@ -1958,7 +1958,7 @@
         <v>181</v>
       </c>
       <c r="H24" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SearchSlots_HappyPath</v>
       </c>
       <c r="I24" t="s">
@@ -2028,7 +2028,7 @@
         <v>182</v>
       </c>
       <c r="H26" s="6" t="str">
-        <f t="shared" ref="H26:H32" si="1">C11</f>
+        <f t="shared" ref="H26:H32" si="2">C11</f>
         <v>BookAppointment_HappyPath013</v>
       </c>
       <c r="I26" t="s">
@@ -2062,7 +2062,7 @@
         <v>183</v>
       </c>
       <c r="H27" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>BookAppointment_HappyPath014</v>
       </c>
       <c r="I27" t="s">
@@ -2098,7 +2098,7 @@
         <v>184</v>
       </c>
       <c r="H28" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>BookAppointment_HappyPath015</v>
       </c>
       <c r="I28" t="s">
@@ -2119,7 +2119,7 @@
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>95</v>
@@ -2134,7 +2134,7 @@
         <v>185</v>
       </c>
       <c r="H29" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>BookAppointment_HappyPath016</v>
       </c>
       <c r="I29" t="s">
@@ -2156,7 +2156,7 @@
         <v>208</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>127</v>
@@ -2168,14 +2168,14 @@
         <v>186</v>
       </c>
       <c r="H30" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>BookAppointment_HappyPath017</v>
       </c>
       <c r="I30" t="s">
         <v>102</v>
       </c>
       <c r="J30" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="K30" t="s">
         <v>121</v>
@@ -2187,7 +2187,7 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>65</v>
@@ -2202,7 +2202,7 @@
         <v>187</v>
       </c>
       <c r="H31" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>BookAppointment_HappyPath018</v>
       </c>
       <c r="I31" t="s">
@@ -2236,7 +2236,7 @@
         <v>188</v>
       </c>
       <c r="H32" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>BookAppointment_HappyPath019</v>
       </c>
       <c r="I32" t="s">
@@ -2255,7 +2255,7 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>91</v>
@@ -2267,7 +2267,7 @@
         <v>92</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
@@ -2294,25 +2294,25 @@
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
+        <v>215</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" t="s">
         <v>218</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="H41" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="H41" s="6" t="s">
+      <c r="I41" t="s">
         <v>221</v>
-      </c>
-      <c r="I41" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="42" spans="2:12" ht="30" x14ac:dyDescent="0.25">
@@ -2342,20 +2342,20 @@
     </row>
     <row r="44" spans="2:12" ht="90" x14ac:dyDescent="0.25">
       <c r="D44" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
+        <v>215</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="47" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>155</v>
@@ -2378,7 +2378,7 @@
     </row>
     <row r="51" spans="4:4" ht="30" x14ac:dyDescent="0.25">
       <c r="D51" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2872,7 +2872,7 @@
         <v>86</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>

</xml_diff>